<commit_message>
get rid of the test data
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Additional_Data_Mapping_Document.xlsx
+++ b/mapping_spreadsheet/Additional_Data_Mapping_Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112B9EEA-9F6C-5746-BAA2-A65CE5052E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C02C871-E6FA-D247-9EEB-82681F7542DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22620" yWindow="8760" windowWidth="27240" windowHeight="16440" xr2:uid="{3863F005-E057-A640-B7EB-01C3C72AEDA2}"/>
   </bookViews>
@@ -67,25 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
-  <si>
-    <t>PAT</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>Term Date</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Forename</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>casrec_table</t>
   </si>
@@ -99,25 +81,10 @@
     <t>sirius_table</t>
   </si>
   <si>
-    <t>persons</t>
-  </si>
-  <si>
-    <t>clients</t>
-  </si>
-  <si>
-    <t>birthdate</t>
-  </si>
-  <si>
     <t>sirius_table_pk_column</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>conditions</t>
-  </si>
-  <si>
-    <t>type=actor_client</t>
   </si>
   <si>
     <t>sirius_alias</t>
@@ -488,148 +455,57 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>